<commit_message>
EPBDS-12729 Remove args parameters because based on discussion it's required for now
</commit_message>
<xml_diff>
--- a/ITEST/itest.WebService/openl-repository/EPBDS-12729/EPBDS-12729/Main.xlsx
+++ b/ITEST/itest.WebService/openl-repository/EPBDS-12729/EPBDS-12729/Main.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpikus/Sources/OpenL/openl-tablets/ITEST/itest.WebService/openl-repository/EPBDS-12729/EPBDS-12729/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2D6654-4B16-FC45-9E5F-61530F4CA6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F793D7BE-1E63-474F-9AF1-F3025AA52445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="34940" windowHeight="22500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>Spreadsheet SpreadsheetResult error1()</t>
   </si>
@@ -34,25 +34,19 @@
     <t>Step1</t>
   </si>
   <si>
-    <t>= error("foo.bar", "Foo bar", 1, 2, 3)</t>
-  </si>
-  <si>
     <t>Spreadsheet SpreadsheetResult error2()</t>
   </si>
   <si>
-    <t>= error("foo.bar", null, 1, 2, 3)</t>
-  </si>
-  <si>
     <t>= error("foo.bar", null)</t>
   </si>
   <si>
     <t>Spreadsheet SpreadsheetResult error3()</t>
   </si>
   <si>
-    <t>Spreadsheet SpreadsheetResult error4()</t>
-  </si>
-  <si>
     <t>= error(null, "Foo bar")</t>
+  </si>
+  <si>
+    <t>= error("foo.bar", "Foo bar")</t>
   </si>
 </sst>
 </file>
@@ -429,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C4:D25"/>
+  <dimension ref="C4:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -478,12 +472,12 @@
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.15">
       <c r="C10" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" s="2"/>
     </row>
@@ -500,59 +494,36 @@
         <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.15">
+      <c r="C20" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C16" t="s">
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.15">
+      <c r="C21" t="s">
         <v>1</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D21" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C17" t="s">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.15">
+      <c r="C22" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C23" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C25" t="s">
-        <v>3</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C20:D20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>